<commit_message>
add marker set / marker template
</commit_message>
<xml_diff>
--- a/server/task/task-spec.xlsx
+++ b/server/task/task-spec.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -36,19 +36,28 @@
     <t>id</t>
   </si>
   <si>
-    <t>Example</t>
-  </si>
-  <si>
     <t>hi</t>
   </si>
   <si>
     <t>{"inputs":[{"name":"Gamma Ray"}],"parameters":[{"name":"GR clean","type":"number","value":10},{"name":"GR clay","type":"number","value":120},{"name":"Method","type":"select","choices":[{"name":"Linear","value":1},{"name":"Clavier","value":2},{"name":"Larionov Tertiary rocks","value":3},{"name":"Larionov older rocks","value":4},{"name":"Stieber variation I","value":5},{"name":"Stieber - Miocene and Pliocene","value":6},{"name":"Stieber variation II","value":7}]}],"outputs":[{"name":"VCL_GR","family":"Clay Volume"}],"function":"calVCLfromGR"}</t>
   </si>
   <si>
-    <t>Example 2</t>
-  </si>
-  <si>
     <t>{"inputs":[{"name":"Bulk Density"},{"name":"Clay Volume"}],"parameters":[{"name":"Bulk Density clean","type":"number","value":2.65},{"name":"Bulk Density fluid","type":"number","value":1},{"name":"Bulk Density clay","type":"number","value":2.3}],"outputs":[{"name":"PHIT_D","family":"Total Porosity"},{"name":"PHIE_D","family":"Effective Porosity"}],"function":"calPorosityFromDensity"}</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>Gamma Ray</t>
+  </si>
+  <si>
+    <t>Clay Volume</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Porosity</t>
   </si>
 </sst>
 </file>
@@ -366,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -376,12 +385,13 @@
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="69.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -389,46 +399,55 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
     </row>

</xml_diff>